<commit_message>
remove middle directory "mtf, sfr, tp1,tp2"
Signed-off-by: Jim Lin <jim_lin@quantatw.com>
</commit_message>
<xml_diff>
--- a/ey3_factory.xlsx
+++ b/ey3_factory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="125">
   <si>
     <t>ROI_0_MTF</t>
   </si>
@@ -388,10 +388,7 @@
     <t>COLOR_YELLOW_DELTA_E</t>
   </si>
   <si>
-    <t>EY3_5006</t>
-  </si>
-  <si>
-    <t>EY3_5004</t>
+    <t>BEY3_5006</t>
   </si>
 </sst>
 </file>
@@ -728,7 +725,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DU3"/>
+  <dimension ref="A1:DU2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1487,383 +1484,6 @@
         <v>75.62611084540001</v>
       </c>
     </row>
-    <row r="3" spans="1:125">
-      <c r="A3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.527</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.766</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.743</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.241</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.765</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.752</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.754</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.423</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.261</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.472</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.329</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.792</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.796</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.799</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.6909999999999999</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0.599</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0.229</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0.49833</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0.440698</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0.493461</v>
-      </c>
-      <c r="W3" t="n">
-        <v>0.460782</v>
-      </c>
-      <c r="X3" t="n">
-        <v>0.456635</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>0.216101</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>0.387502</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>0.228025</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>0.557071</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>0.550083</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>0.546194</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>0.500224</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>0.463905</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>0.26445</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>0.518495</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>0.456694</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>0.487521</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>0.558382</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>0.463638</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>0.442755</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>0.573627</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>0.5197040000000001</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>0.477584</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>0.503978</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>0.421123</v>
-      </c>
-      <c r="AS3" t="n">
-        <v>0.254311</v>
-      </c>
-      <c r="AT3" t="n">
-        <v>0.283036</v>
-      </c>
-      <c r="AU3" t="n">
-        <v>0.418754</v>
-      </c>
-      <c r="AV3" t="n">
-        <v>0.498097</v>
-      </c>
-      <c r="AW3" t="n">
-        <v>0.440176</v>
-      </c>
-      <c r="AX3" t="n">
-        <v>0.429538</v>
-      </c>
-      <c r="AY3" t="n">
-        <v>0.45382</v>
-      </c>
-      <c r="AZ3" t="n">
-        <v>0.213983</v>
-      </c>
-      <c r="BA3" t="n">
-        <v>0.217168</v>
-      </c>
-      <c r="BB3" t="n">
-        <v>0.226824</v>
-      </c>
-      <c r="BC3" t="n">
-        <v>0.241447</v>
-      </c>
-      <c r="BD3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BI3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BJ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BK3" t="n">
-        <v>0.442763</v>
-      </c>
-      <c r="BL3" t="n">
-        <v>0.482411</v>
-      </c>
-      <c r="BM3" t="n">
-        <v>0.481756</v>
-      </c>
-      <c r="BN3" t="n">
-        <v>0.488117</v>
-      </c>
-      <c r="BO3" t="n">
-        <v>0.466793</v>
-      </c>
-      <c r="BP3" t="n">
-        <v>0.425578</v>
-      </c>
-      <c r="BQ3" t="n">
-        <v>0.459726</v>
-      </c>
-      <c r="BR3" t="n">
-        <v>0.459943</v>
-      </c>
-      <c r="BS3" t="n">
-        <v>0.466246</v>
-      </c>
-      <c r="BT3" t="n">
-        <v>0.446127</v>
-      </c>
-      <c r="BU3" t="n">
-        <v>0.412856</v>
-      </c>
-      <c r="BV3" t="n">
-        <v>0.448792</v>
-      </c>
-      <c r="BW3" t="n">
-        <v>0.447507</v>
-      </c>
-      <c r="BX3" t="n">
-        <v>0.454162</v>
-      </c>
-      <c r="BY3" t="n">
-        <v>0.433999</v>
-      </c>
-      <c r="BZ3" t="n">
-        <v>0.397335</v>
-      </c>
-      <c r="CA3" t="n">
-        <v>0.425996</v>
-      </c>
-      <c r="CB3" t="n">
-        <v>0.426248</v>
-      </c>
-      <c r="CC3" t="n">
-        <v>0.43207</v>
-      </c>
-      <c r="CD3" t="n">
-        <v>0.414025</v>
-      </c>
-      <c r="CE3" t="n">
-        <v>1.01393</v>
-      </c>
-      <c r="CF3" t="n">
-        <v>1.010218</v>
-      </c>
-      <c r="CG3" t="n">
-        <v>0.9963379999999999</v>
-      </c>
-      <c r="CH3" t="n">
-        <v>0.91972</v>
-      </c>
-      <c r="CI3" t="n">
-        <v>0.92782</v>
-      </c>
-      <c r="CJ3" t="n">
-        <v>1.008807</v>
-      </c>
-      <c r="CK3" t="n">
-        <v>0.925492</v>
-      </c>
-      <c r="CL3" t="n">
-        <v>0.93496</v>
-      </c>
-      <c r="CM3" t="n">
-        <v>1.010229</v>
-      </c>
-      <c r="CN3" t="n">
-        <v>0.921714</v>
-      </c>
-      <c r="CO3" t="n">
-        <v>0.930658</v>
-      </c>
-      <c r="CP3" t="n">
-        <v>1.009704</v>
-      </c>
-      <c r="CQ3" t="n">
-        <v>0.932418</v>
-      </c>
-      <c r="CR3" t="n">
-        <v>0.9419729999999999</v>
-      </c>
-      <c r="CS3" t="n">
-        <v>1.010247</v>
-      </c>
-      <c r="CT3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CU3" t="n">
-        <v>2036</v>
-      </c>
-      <c r="CV3" t="n">
-        <v>1459</v>
-      </c>
-      <c r="CW3" t="n">
-        <v>43</v>
-      </c>
-      <c r="CX3" t="n">
-        <v>-16</v>
-      </c>
-      <c r="CY3" t="n">
-        <v>45.880279</v>
-      </c>
-      <c r="CZ3" t="n">
-        <v>-0.7726730000000001</v>
-      </c>
-      <c r="DA3" t="n">
-        <v>-5.438497</v>
-      </c>
-      <c r="DB3" t="n">
-        <v>-11.354755</v>
-      </c>
-      <c r="DC3" t="n">
-        <v>28.991037</v>
-      </c>
-      <c r="DD3" t="n">
-        <v>51.423973</v>
-      </c>
-      <c r="DE3" t="n">
-        <v>49.828533</v>
-      </c>
-      <c r="DF3" t="n">
-        <v>34.654961</v>
-      </c>
-      <c r="DG3" t="n">
-        <v>36.91346</v>
-      </c>
-      <c r="DH3" t="n">
-        <v>21.606945</v>
-      </c>
-      <c r="DI3" t="n">
-        <v>-1.699978</v>
-      </c>
-      <c r="DJ3" t="n">
-        <v>21.6082770267</v>
-      </c>
-      <c r="DK3" t="n">
-        <v>44.5669267772</v>
-      </c>
-      <c r="DL3" t="n">
-        <v>7.7825932706</v>
-      </c>
-      <c r="DM3" t="n">
-        <v>36.6429585954</v>
-      </c>
-      <c r="DN3" t="n">
-        <v>12.7551762383</v>
-      </c>
-      <c r="DO3" t="n">
-        <v>37.3164289969</v>
-      </c>
-      <c r="DP3" t="n">
-        <v>16.599634194</v>
-      </c>
-      <c r="DQ3" t="n">
-        <v>58.0546819261</v>
-      </c>
-      <c r="DR3" t="n">
-        <v>21.1972484955</v>
-      </c>
-      <c r="DS3" t="n">
-        <v>46.3878381336</v>
-      </c>
-      <c r="DT3" t="n">
-        <v>21.7536413072</v>
-      </c>
-      <c r="DU3" t="n">
-        <v>78.3309545784</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>